<commit_message>
Added Displays + Sudoku Regions & UI tweaks
Faltan
> 5x5
> 7x7
> 11x11
> 13x13
> 17x17
> 19x19
</commit_message>
<xml_diff>
--- a/Tamaños de sudoku.xlsx
+++ b/Tamaños de sudoku.xlsx
@@ -97,15 +97,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -113,12 +119,119 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,13 +639,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>91440</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>327660</xdr:rowOff>
     </xdr:to>
@@ -558,7 +671,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9098280" y="3657600"/>
+          <a:off x="9189720" y="3657600"/>
           <a:ext cx="2849880" cy="2880360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -745,14 +858,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>383683</xdr:colOff>
+      <xdr:colOff>437023</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
@@ -778,7 +891,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7322820" y="7299960"/>
+          <a:off x="7376160" y="7307580"/>
           <a:ext cx="3058303" cy="3131820"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -808,8 +921,8 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>5892</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>188772</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -911,15 +1024,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -943,7 +1056,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4511040" y="10980420"/>
+          <a:off x="4587240" y="10972800"/>
           <a:ext cx="4099560" cy="4099560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1289,10 +1402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Y65"/>
+  <dimension ref="A1:AB65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V48" sqref="V48"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21:V39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1319,80 +1432,1581 @@
     <col min="23" max="23" width="6.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:27" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T1" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="2:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:25" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:25" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="12"/>
+    </row>
+    <row r="2" spans="1:27" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="15"/>
+    </row>
+    <row r="3" spans="1:27" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="15"/>
+    </row>
+    <row r="4" spans="1:27" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="15"/>
+    </row>
+    <row r="5" spans="1:27" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="15"/>
+    </row>
+    <row r="6" spans="1:27" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="15"/>
+    </row>
+    <row r="7" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="15"/>
+    </row>
+    <row r="8" spans="1:27" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="18"/>
+    </row>
+    <row r="9" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:27" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G10" t="s">
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M10" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="T10" t="s">
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="2:25" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:25" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:25" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:24" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:24" ht="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:24" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="3"/>
+    </row>
+    <row r="11" spans="1:27" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="6"/>
+    </row>
+    <row r="12" spans="1:27" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="6"/>
+    </row>
+    <row r="13" spans="1:27" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="6"/>
+    </row>
+    <row r="14" spans="1:27" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="6"/>
+    </row>
+    <row r="16" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="6"/>
+    </row>
+    <row r="17" spans="1:28" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="6"/>
+    </row>
+    <row r="18" spans="1:28" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="9"/>
+    </row>
+    <row r="19" spans="1:28" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I21" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P21" t="s">
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="3"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="6"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="6"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="6"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="6"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="14"/>
+      <c r="U26" s="14"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="6"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+      <c r="U27" s="14"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="6"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+      <c r="U28" s="14"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="6"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14"/>
+      <c r="T29" s="14"/>
+      <c r="U29" s="14"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="6"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+      <c r="U30" s="14"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="6"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="15"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="6"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="14"/>
+      <c r="U32" s="14"/>
+      <c r="V32" s="15"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="6"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="14"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="15"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="6"/>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="14"/>
+      <c r="V34" s="15"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="5"/>
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="5"/>
+      <c r="AB34" s="6"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="6"/>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="6"/>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="6"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A38" s="13"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="15"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="5"/>
+      <c r="Y38" s="5"/>
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="6"/>
+    </row>
+    <row r="39" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="16"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="18"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="5"/>
+      <c r="Y39" s="5"/>
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="6"/>
+    </row>
+    <row r="40" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W40" s="7"/>
+      <c r="X40" s="8"/>
+      <c r="Y40" s="8"/>
+      <c r="Z40" s="8"/>
+      <c r="AA40" s="8"/>
+      <c r="AB40" s="9"/>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J41" t="s">
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="3"/>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A42" s="13"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="6"/>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A43" s="13"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="6"/>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A44" s="13"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="6"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="6"/>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A46" s="13"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="6"/>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A47" s="13"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="6"/>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A48" s="13"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="6"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="13"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="6"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="13"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="6"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" s="13"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="6"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" s="13"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="6"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="13"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="6"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="13"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="6"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="13"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="6"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="6"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A57" s="13"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="S57" s="6"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A58" s="13"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="6"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A59" s="13"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="6"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A60" s="13"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="5"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="5"/>
+      <c r="S60" s="6"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A61" s="13"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="6"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A62" s="13"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5"/>
+      <c r="P62" s="5"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="5"/>
+      <c r="S62" s="6"/>
+    </row>
+    <row r="63" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="16"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
+      <c r="P63" s="5"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="5"/>
+      <c r="S63" s="6"/>
+    </row>
+    <row r="64" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>16</v>
       </c>
+      <c r="J64" s="7"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="8"/>
+      <c r="M64" s="8"/>
+      <c r="N64" s="8"/>
+      <c r="O64" s="8"/>
+      <c r="P64" s="8"/>
+      <c r="Q64" s="8"/>
+      <c r="R64" s="8"/>
+      <c r="S64" s="9"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
@@ -1401,7 +3015,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Sudoku Saving & other fixes
</commit_message>
<xml_diff>
--- a/Tamaños de sudoku.xlsx
+++ b/Tamaños de sudoku.xlsx
@@ -254,15 +254,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -286,7 +286,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="502920" y="419100"/>
+          <a:off x="685800" y="449580"/>
           <a:ext cx="1927860" cy="1813560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -309,15 +309,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>365760</xdr:rowOff>
+      <xdr:rowOff>373380</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -341,7 +341,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3002280" y="373380"/>
+          <a:off x="3078480" y="381000"/>
           <a:ext cx="2270760" cy="2156460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -364,15 +364,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>365760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:colOff>403860</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
+      <xdr:rowOff>320040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -396,7 +396,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5996940" y="388620"/>
+          <a:off x="5989320" y="365760"/>
           <a:ext cx="2613660" cy="2499360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -419,15 +419,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>213360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -451,7 +451,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9098280" y="373380"/>
+          <a:off x="9311640" y="381000"/>
           <a:ext cx="2049780" cy="2087880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -473,16 +473,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>739140</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>335280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>243840</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -506,7 +506,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11643360" y="388620"/>
+          <a:off x="12024360" y="335280"/>
           <a:ext cx="2400300" cy="2400300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1024,15 +1024,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:colOff>182880</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1056,7 +1056,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4587240" y="10972800"/>
+          <a:off x="4724400" y="11003280"/>
           <a:ext cx="4099560" cy="4099560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1404,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21:V39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1432,14 +1432,14 @@
     <col min="23" max="23" width="6.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:28" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
       <c r="G1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1468,14 +1468,15 @@
         <v>4</v>
       </c>
       <c r="Z1" s="11"/>
-      <c r="AA1" s="12"/>
-    </row>
-    <row r="2" spans="1:27" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="12"/>
+    </row>
+    <row r="2" spans="1:28" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="13"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -1496,14 +1497,15 @@
       <c r="X2" s="15"/>
       <c r="Y2" s="13"/>
       <c r="Z2" s="14"/>
-      <c r="AA2" s="15"/>
-    </row>
-    <row r="3" spans="1:27" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="15"/>
+    </row>
+    <row r="3" spans="1:28" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="13"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -1524,14 +1526,15 @@
       <c r="X3" s="15"/>
       <c r="Y3" s="13"/>
       <c r="Z3" s="14"/>
-      <c r="AA3" s="15"/>
-    </row>
-    <row r="4" spans="1:27" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="15"/>
+    </row>
+    <row r="4" spans="1:28" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="13"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -1552,14 +1555,15 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="13"/>
       <c r="Z4" s="14"/>
-      <c r="AA4" s="15"/>
-    </row>
-    <row r="5" spans="1:27" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="15"/>
+    </row>
+    <row r="5" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="13"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -1580,14 +1584,15 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="13"/>
       <c r="Z5" s="14"/>
-      <c r="AA5" s="15"/>
-    </row>
-    <row r="6" spans="1:27" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="15"/>
+    </row>
+    <row r="6" spans="1:28" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="13"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -1608,14 +1613,15 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="13"/>
       <c r="Z6" s="14"/>
-      <c r="AA6" s="15"/>
-    </row>
-    <row r="7" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="15"/>
+    </row>
+    <row r="7" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="13"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -1636,14 +1642,15 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
       <c r="Z7" s="14"/>
-      <c r="AA7" s="15"/>
-    </row>
-    <row r="8" spans="1:27" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="15"/>
+    </row>
+    <row r="8" spans="1:28" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="16"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
@@ -1664,10 +1671,11 @@
       <c r="X8" s="18"/>
       <c r="Y8" s="16"/>
       <c r="Z8" s="17"/>
-      <c r="AA8" s="18"/>
-    </row>
-    <row r="9" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:27" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="18"/>
+    </row>
+    <row r="9" spans="1:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:28" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
       <c r="B10" s="20" t="s">
         <v>5</v>
@@ -1702,7 +1710,7 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="3"/>
     </row>
-    <row r="11" spans="1:27" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -1729,7 +1737,7 @@
       <c r="X11" s="5"/>
       <c r="Y11" s="6"/>
     </row>
-    <row r="12" spans="1:27" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -1756,7 +1764,7 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="6"/>
     </row>
-    <row r="13" spans="1:27" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -1783,7 +1791,7 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="6"/>
     </row>
-    <row r="14" spans="1:27" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -1810,7 +1818,7 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="6"/>
     </row>
-    <row r="15" spans="1:27" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -1837,7 +1845,7 @@
       <c r="X15" s="5"/>
       <c r="Y15" s="6"/>
     </row>
-    <row r="16" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -3025,7 +3033,7 @@
   <dimension ref="A2:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Bugfixes, UI tweaks & Testing Gen (5-10)
</commit_message>
<xml_diff>
--- a/Tamaños de sudoku.xlsx
+++ b/Tamaños de sudoku.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13200" windowHeight="6168" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13200" windowHeight="6168" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sudokus" sheetId="1" r:id="rId1"/>
     <sheet name="Formas tetris" sheetId="2" r:id="rId2"/>
+    <sheet name="Tests" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>5x5</t>
   </si>
@@ -106,13 +107,106 @@
   </si>
   <si>
     <t>Testing grid</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Gen 1</t>
+  </si>
+  <si>
+    <t>Gen 2</t>
+  </si>
+  <si>
+    <t>Gen 3</t>
+  </si>
+  <si>
+    <t>Solve 1</t>
+  </si>
+  <si>
+    <t>Solve 2</t>
+  </si>
+  <si>
+    <t>Solve 3</t>
+  </si>
+  <si>
+    <t>Tiempo (main thread)</t>
+  </si>
+  <si>
+    <t>Numero threads para solver</t>
+  </si>
+  <si>
+    <t>Se esta usando el que haya durado menos en el main thread</t>
+  </si>
+  <si>
+    <t>entre los 3 generados</t>
+  </si>
+  <si>
+    <t>no regions</t>
+  </si>
+  <si>
+    <t>00:25.85</t>
+  </si>
+  <si>
+    <t>00:15.07</t>
+  </si>
+  <si>
+    <t>00:25.43</t>
+  </si>
+  <si>
+    <t>00:12.14</t>
+  </si>
+  <si>
+    <t>00:08.05</t>
+  </si>
+  <si>
+    <t>00:11.55</t>
+  </si>
+  <si>
+    <t>00:13.80</t>
+  </si>
+  <si>
+    <t>00:14.61</t>
+  </si>
+  <si>
+    <t>00:15.71</t>
+  </si>
+  <si>
+    <t>00:30.79</t>
+  </si>
+  <si>
+    <t>00:35.86</t>
+  </si>
+  <si>
+    <t>NO TIENE PUNTITOS</t>
+  </si>
+  <si>
+    <t>00:18.90</t>
+  </si>
+  <si>
+    <t>00:29.14</t>
+  </si>
+  <si>
+    <t>00:44.45</t>
+  </si>
+  <si>
+    <t>00:54.51</t>
+  </si>
+  <si>
+    <t>01:23.98</t>
+  </si>
+  <si>
+    <t>00:38.55</t>
+  </si>
+  <si>
+    <t>01:05.26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,8 +214,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,8 +241,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -324,11 +461,121 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -387,6 +634,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3188,7 +3495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -3296,4 +3603,561 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30"/>
+      <c r="B1" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="43">
+        <v>5</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="39">
+        <v>6</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="J4" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="58"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="39">
+        <v>7</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="39">
+        <v>8</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="39">
+        <v>9</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="39">
+        <v>10</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="39">
+        <v>11</v>
+      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="39">
+        <v>12</v>
+      </c>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="39">
+        <v>13</v>
+      </c>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="39">
+        <v>14</v>
+      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="39">
+        <v>15</v>
+      </c>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="39">
+        <v>16</v>
+      </c>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="39">
+        <v>17</v>
+      </c>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="39">
+        <v>18</v>
+      </c>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="40">
+        <v>19</v>
+      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="30"/>
+      <c r="B21" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="48"/>
+      <c r="M21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="50">
+        <v>1</v>
+      </c>
+      <c r="C22" s="50">
+        <v>2</v>
+      </c>
+      <c r="D22" s="50">
+        <v>3</v>
+      </c>
+      <c r="E22" s="50">
+        <v>4</v>
+      </c>
+      <c r="F22" s="50">
+        <v>5</v>
+      </c>
+      <c r="G22" s="50">
+        <v>6</v>
+      </c>
+      <c r="H22" s="50">
+        <v>7</v>
+      </c>
+      <c r="I22" s="50">
+        <v>8</v>
+      </c>
+      <c r="J22" s="50">
+        <v>9</v>
+      </c>
+      <c r="K22" s="50">
+        <v>10</v>
+      </c>
+      <c r="M22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="51">
+        <v>5</v>
+      </c>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="52">
+        <v>6</v>
+      </c>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="52">
+        <v>7</v>
+      </c>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="52">
+        <v>8</v>
+      </c>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="52">
+        <v>9</v>
+      </c>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="52">
+        <v>10</v>
+      </c>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="52">
+        <v>11</v>
+      </c>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="52">
+        <v>12</v>
+      </c>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="52">
+        <v>13</v>
+      </c>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="52">
+        <v>14</v>
+      </c>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="52"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="52">
+        <v>15</v>
+      </c>
+      <c r="B33" s="52"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="52"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="52">
+        <v>16</v>
+      </c>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="52">
+        <v>17</v>
+      </c>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="52">
+        <v>18</v>
+      </c>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+    </row>
+    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="53">
+        <v>19</v>
+      </c>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="J4:K4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>